<commit_message>
patent diagrams are added
</commit_message>
<xml_diff>
--- a/new_modules/Summary_2022-06-09_L2A.xlsx
+++ b/new_modules/Summary_2022-06-09_L2A.xlsx
@@ -441,19 +441,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>-0.1562</v>
+        <v>0.9067</v>
       </c>
       <c r="C2">
-        <v>-0.1562</v>
+        <v>0.9067</v>
       </c>
       <c r="D2">
-        <v>-0.1643</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0.1111</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>-0.5402</v>
+        <v>0.5798</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -461,19 +461,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>-0.1712</v>
+        <v>0.992</v>
       </c>
       <c r="C3">
-        <v>-0.1712</v>
+        <v>0.992</v>
       </c>
       <c r="D3">
-        <v>-0.1764</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0.2046</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>-0.4198</v>
+        <v>0.8033</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -481,19 +481,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>-0.0896</v>
+        <v>0.9896</v>
       </c>
       <c r="C4">
-        <v>-0.0896</v>
+        <v>0.9896</v>
       </c>
       <c r="D4">
-        <v>-0.08069999999999999</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0.1335</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>-0.3636</v>
+        <v>0.8442</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -501,19 +501,19 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.0517</v>
+        <v>0.9874000000000001</v>
       </c>
       <c r="C5">
-        <v>0.0517</v>
+        <v>0.9874000000000001</v>
       </c>
       <c r="D5">
-        <v>0.0586</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0.2607</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>-0.2958</v>
+        <v>0.8874</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -521,19 +521,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0.0512</v>
+        <v>0.9791</v>
       </c>
       <c r="C6">
-        <v>0.0512</v>
+        <v>0.9791</v>
       </c>
       <c r="D6">
-        <v>0.0456</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>0.2034</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>-0.3402</v>
+        <v>0.8509</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -541,19 +541,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>0.0503</v>
+        <v>0.9715</v>
       </c>
       <c r="C7">
-        <v>0.0503</v>
+        <v>0.9715</v>
       </c>
       <c r="D7">
-        <v>0.0444</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>0.1801</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>-0.1017</v>
+        <v>0.8243</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -561,19 +561,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>0.0842</v>
+        <v>0.9471000000000001</v>
       </c>
       <c r="C8">
-        <v>0.0842</v>
+        <v>0.9471000000000001</v>
       </c>
       <c r="D8">
-        <v>0.07829999999999999</v>
+        <v>0.9494</v>
       </c>
       <c r="E8">
-        <v>0.214</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>-0.143</v>
+        <v>0.8022</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new SMS sending module folder
</commit_message>
<xml_diff>
--- a/new_modules/Summary_2022-06-09_L2A.xlsx
+++ b/new_modules/Summary_2022-06-09_L2A.xlsx
@@ -441,19 +441,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0.9067</v>
+        <v>-0.1562</v>
       </c>
       <c r="C2">
-        <v>0.9067</v>
+        <v>-0.1562</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>-0.1643</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0.1111</v>
       </c>
       <c r="F2">
-        <v>0.5798</v>
+        <v>-0.5402</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -461,19 +461,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.992</v>
+        <v>-0.1712</v>
       </c>
       <c r="C3">
-        <v>0.992</v>
+        <v>-0.1712</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>-0.1764</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0.2046</v>
       </c>
       <c r="F3">
-        <v>0.8033</v>
+        <v>-0.4198</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -481,19 +481,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0.9896</v>
+        <v>-0.0896</v>
       </c>
       <c r="C4">
-        <v>0.9896</v>
+        <v>-0.0896</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>-0.08069999999999999</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0.1335</v>
       </c>
       <c r="F4">
-        <v>0.8442</v>
+        <v>-0.3636</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -501,19 +501,19 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.9874000000000001</v>
+        <v>0.0517</v>
       </c>
       <c r="C5">
-        <v>0.9874000000000001</v>
+        <v>0.0517</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0.0586</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0.2607</v>
       </c>
       <c r="F5">
-        <v>0.8874</v>
+        <v>-0.2958</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -521,19 +521,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0.9791</v>
+        <v>0.0512</v>
       </c>
       <c r="C6">
-        <v>0.9791</v>
+        <v>0.0512</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0.0456</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0.2034</v>
       </c>
       <c r="F6">
-        <v>0.8509</v>
+        <v>-0.3402</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -541,19 +541,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>0.9715</v>
+        <v>0.0503</v>
       </c>
       <c r="C7">
-        <v>0.9715</v>
+        <v>0.0503</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0.0444</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0.1801</v>
       </c>
       <c r="F7">
-        <v>0.8243</v>
+        <v>-0.1017</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -561,19 +561,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>0.9471000000000001</v>
+        <v>0.0842</v>
       </c>
       <c r="C8">
-        <v>0.9471000000000001</v>
+        <v>0.0842</v>
       </c>
       <c r="D8">
-        <v>0.9494</v>
+        <v>0.07829999999999999</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0.214</v>
       </c>
       <c r="F8">
-        <v>0.8022</v>
+        <v>-0.143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
K means clustering is applied
</commit_message>
<xml_diff>
--- a/new_modules/Summary_2022-06-09_L2A.xlsx
+++ b/new_modules/Summary_2022-06-09_L2A.xlsx
@@ -441,19 +441,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>-0.1562</v>
+        <v>0.4914</v>
       </c>
       <c r="C2">
-        <v>-0.1562</v>
+        <v>0.4914</v>
       </c>
       <c r="D2">
-        <v>-0.1643</v>
+        <v>0.5338000059127808</v>
       </c>
       <c r="E2">
-        <v>0.1111</v>
+        <v>0.9686999917030334</v>
       </c>
       <c r="F2">
-        <v>-0.5402</v>
+        <v>0.1958000063896179</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -461,19 +461,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>-0.1712</v>
+        <v>0.5916</v>
       </c>
       <c r="C3">
-        <v>-0.1712</v>
+        <v>0.5916</v>
       </c>
       <c r="D3">
-        <v>-0.1764</v>
+        <v>0.6016</v>
       </c>
       <c r="E3">
-        <v>0.2046</v>
+        <v>0.8482999801635742</v>
       </c>
       <c r="F3">
-        <v>-0.4198</v>
+        <v>0.2239000052213669</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -481,19 +481,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>-0.0896</v>
+        <v>0.5077</v>
       </c>
       <c r="C4">
-        <v>-0.0896</v>
+        <v>0.5077</v>
       </c>
       <c r="D4">
-        <v>-0.08069999999999999</v>
+        <v>0.508</v>
       </c>
       <c r="E4">
-        <v>0.1335</v>
+        <v>0.7921000123023987</v>
       </c>
       <c r="F4">
-        <v>-0.3636</v>
+        <v>0.2542999982833862</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -501,19 +501,19 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.0517</v>
+        <v>0.3642</v>
       </c>
       <c r="C5">
-        <v>0.0517</v>
+        <v>0.3642</v>
       </c>
       <c r="D5">
-        <v>0.0586</v>
+        <v>0.361</v>
       </c>
       <c r="E5">
-        <v>0.2607</v>
+        <v>0.7243000268936157</v>
       </c>
       <c r="F5">
-        <v>-0.2958</v>
+        <v>0.1677999943494797</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -521,19 +521,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0.0512</v>
+        <v>0.3564</v>
       </c>
       <c r="C6">
-        <v>0.0512</v>
+        <v>0.3564</v>
       </c>
       <c r="D6">
-        <v>0.0456</v>
+        <v>0.3484</v>
       </c>
       <c r="E6">
-        <v>0.2034</v>
+        <v>0.7688000202178955</v>
       </c>
       <c r="F6">
-        <v>-0.3402</v>
+        <v>0.2064000070095062</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -541,19 +541,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>0.0503</v>
+        <v>0.3497</v>
       </c>
       <c r="C7">
-        <v>0.0503</v>
+        <v>0.3497</v>
       </c>
       <c r="D7">
-        <v>0.0444</v>
+        <v>0.3607000112533569</v>
       </c>
       <c r="E7">
-        <v>0.1801</v>
+        <v>0.5302000045776367</v>
       </c>
       <c r="F7">
-        <v>-0.1017</v>
+        <v>0.2302999943494797</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -561,19 +561,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>0.0842</v>
+        <v>0.2914</v>
       </c>
       <c r="C8">
-        <v>0.0842</v>
+        <v>0.2914</v>
       </c>
       <c r="D8">
-        <v>0.07829999999999999</v>
+        <v>0.28</v>
       </c>
       <c r="E8">
-        <v>0.214</v>
+        <v>0.4905000030994415</v>
       </c>
       <c r="F8">
-        <v>-0.143</v>
+        <v>0.214599996805191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ground data for 3 years
</commit_message>
<xml_diff>
--- a/new_modules/Summary_2022-06-09_L2A.xlsx
+++ b/new_modules/Summary_2022-06-09_L2A.xlsx
@@ -444,19 +444,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>1.141199946403503</v>
+        <v>-278.434814453125</v>
       </c>
       <c r="C2">
-        <v>0.0009</v>
+        <v>-0.2089</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.0071000000461936</v>
       </c>
       <c r="E2">
-        <v>0.3989000022411346</v>
+        <v>0.1920000016689301</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>-1.067000031471252</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -464,19 +464,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.4153999984264374</v>
+        <v>17.83259963989258</v>
       </c>
       <c r="C3">
-        <v>0.0003</v>
+        <v>0.0143</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.0353</v>
       </c>
       <c r="E3">
-        <v>0.06069999933242798</v>
+        <v>0.1861000061035156</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>-0.5751000046730042</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -484,19 +484,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>-2.079600095748901</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>-0.0024</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.0186</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.1064999997615814</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>-0.3657000064849854</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -504,19 +504,19 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>53.41999816894531</v>
+        <v>66.30210113525391</v>
       </c>
       <c r="C5">
-        <v>0.0564</v>
+        <v>0.0699</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.0398</v>
       </c>
       <c r="E5">
-        <v>0.7074999809265137</v>
+        <v>0.8353999853134155</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>-0.2746999859809875</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -524,19 +524,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>113.3384017944336</v>
+        <v>112.2123031616211</v>
       </c>
       <c r="C6">
-        <v>0.0897</v>
+        <v>0.0888</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>0.033</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>1.145699977874756</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>-0.3203000128269196</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -544,19 +544,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>22.33880043029785</v>
+        <v>-6.190400123596191</v>
       </c>
       <c r="C7">
-        <v>0.0225</v>
+        <v>-0.0062</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>0.01820000074803829</v>
       </c>
       <c r="E7">
-        <v>0.5268999934196472</v>
+        <v>0.65420001745224</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>-0.4032999873161316</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -564,19 +564,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>35.45539855957031</v>
+        <v>-51.31719970703125</v>
       </c>
       <c r="C8">
-        <v>0.0318</v>
+        <v>-0.046</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>-0.0607</v>
       </c>
       <c r="E8">
-        <v>0.5268999934196472</v>
+        <v>0.65420001745224</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>-0.4408999979496002</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -584,19 +584,19 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>226.1092071533203</v>
+        <v>-141.6749877929688</v>
       </c>
       <c r="C9">
-        <v>0.029</v>
+        <v>-0.0186</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>0.0257</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>1.145699977874756</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>-1.067000031471252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>